<commit_message>
[FIX] nitrate uptake ratio constraint is now optional + [ADD] other steps to documentation + [MOVE] model files from tests to examples
</commit_message>
<xml_diff>
--- a/validation/arabidopsis/simulation_sp/produced_at_day.xlsx
+++ b/validation/arabidopsis/simulation_sp/produced_at_day.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -458,17 +458,17 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Sucrose_c_Day_sp_exchange</t>
+          <t>Sucrose_c__Day_sp_exchange</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>0.02497</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.2960924999994341</v>
+        <v>-0.296092499999758</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2960924999994431</v>
+        <v>0.2960925000000199</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
@@ -477,7 +477,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>L-Isoleucine_Day_sp_exchange</t>
+          <t>L-Isoleucine__Day_sp_exchange</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -487,7 +487,7 @@
         <v>-0.0033</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0033</v>
+        <v>0.003300000000004672</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -496,17 +496,17 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>L-Leucine_Day_sp_exchange</t>
+          <t>L-Leucine__Day_sp_exchange</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.0077</v>
+        <v>0.007700000000000001</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.0077</v>
+        <v>-0.007700000000000001</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0077</v>
+        <v>0.007700000000000001</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -515,11 +515,11 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>L-Lysine_Day_sp_exchange</t>
+          <t>L-Lysine__Day_sp_exchange</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5.500000000000028e-05</v>
+        <v>5.5e-05</v>
       </c>
       <c r="C5" t="n">
         <v>-5.5e-05</v>
@@ -534,17 +534,17 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>L-Methionine_Day_sp_exchange</t>
+          <t>L-Methionine__Day_sp_exchange</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.00011</v>
+        <v>0.0001100000000000007</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.0001099999999962985</v>
+        <v>-0.0001099999999999973</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0001100000000000028</v>
+        <v>0.0001100000000000007</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -553,17 +553,17 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>L-Phenylalanine_Day_sp_exchange</t>
+          <t>L-Phenylalanine__Day_sp_exchange</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.004400000000000007</v>
+        <v>0.0044</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.02793999999986958</v>
+        <v>-0.02793999999999629</v>
       </c>
       <c r="D7" t="n">
-        <v>0.02794000000000001</v>
+        <v>0.02794000000000039</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -572,17 +572,17 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>L-Threonine_Day_sp_exchange</t>
+          <t>L-Threonine__Day_sp_exchange</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.004729999999999999</v>
+        <v>0.00473</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.01154999999996687</v>
+        <v>-0.01155000000000263</v>
       </c>
       <c r="D8" t="n">
-        <v>0.01155000000000001</v>
+        <v>0.01155</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -591,17 +591,17 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>L-Tryptophan_Day_sp_exchange</t>
+          <t>L-Tryptophan__Day_sp_exchange</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.002200000000000001</v>
+        <v>0.0022</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.002200000000000001</v>
+        <v>-0.0022</v>
       </c>
       <c r="D9" t="n">
-        <v>0.002200000000000001</v>
+        <v>0.0022</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -610,17 +610,17 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>L-Valine_Day_sp_exchange</t>
+          <t>L-Valine__Day_sp_exchange</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.005500000000000002</v>
+        <v>0.005500000000000001</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.02089999999998739</v>
+        <v>-0.0209</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0209</v>
+        <v>0.02090000000001515</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -629,17 +629,17 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>L-Cysteine_Day_sp_exchange</t>
+          <t>L-Cysteine__Day_sp_exchange</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>0.00132</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.00131999999983542</v>
+        <v>-0.001320000000052017</v>
       </c>
       <c r="D11" t="n">
-        <v>0.001319999999866685</v>
+        <v>0.00132</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -648,17 +648,17 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>L-Glutamine_c_Day_sp_exchange</t>
+          <t>L-Glutamine_c__Day_sp_exchange</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.02048200000000043</v>
+        <v>0.02048199999999901</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.192604892856885</v>
+        <v>-0.1926048928569813</v>
       </c>
       <c r="D12" t="n">
-        <v>0.481076749999466</v>
+        <v>0.4810767499997521</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -667,17 +667,17 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>L-Glutamate_c_Day_sp_exchange</t>
+          <t>L-Glutamate_c__Day_sp_exchange</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1.416330230160195</v>
+        <v>1.416330230157635</v>
       </c>
       <c r="C13" t="n">
-        <v>1.203238055555509</v>
+        <v>1.203238055555524</v>
       </c>
       <c r="D13" t="n">
-        <v>7.611845999993817</v>
+        <v>7.611845999994399</v>
       </c>
       <c r="E13" t="b">
         <v>1</v>
@@ -686,17 +686,17 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>L-Tyrosine_Day_sp_exchange</t>
+          <t>L-Tyrosine__Day_sp_exchange</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.009569999999999997</v>
+        <v>0.00957</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.00957</v>
+        <v>-0.009570000000006613</v>
       </c>
       <c r="D14" t="n">
-        <v>0.009569999999983739</v>
+        <v>0.009570000000003095</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -705,17 +705,17 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>L-Asparagine_Day_sp_exchange</t>
+          <t>L-Asparagine__Day_sp_exchange</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>0.02145</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.1488162499998272</v>
+        <v>-0.1488162499999055</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1488162499996062</v>
+        <v>0.1488162500000992</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -724,17 +724,17 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>L-Serine_c_Day_sp_exchange</t>
+          <t>L-Serine_c__Day_sp_exchange</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>0.01155</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.2733224999994143</v>
+        <v>-0.2733225000001817</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2733224999988936</v>
+        <v>0.2733225000001933</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -743,17 +743,17 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>L-Aspartate_c_Day_sp_exchange</t>
+          <t>L-Aspartate_c__Day_sp_exchange</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.2722904206341817</v>
+        <v>0.2722904206358095</v>
       </c>
       <c r="C17" t="n">
-        <v>-4.424533666665673</v>
+        <v>-4.424533666668475</v>
       </c>
       <c r="D17" t="n">
-        <v>0.6158618888881841</v>
+        <v>0.6158618888889418</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
@@ -762,17 +762,17 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Starch_p_Day_sp_exchange</t>
+          <t>Starch_p__Day_sp_exchange</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.1141292777775617</v>
+        <v>0.1141292777779996</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.2856974999984733</v>
+        <v>-0.2856975000007493</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2609575833331929</v>
+        <v>0.2609575833332883</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
@@ -781,17 +781,17 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>(S)-Malate_c_Day_sp_exchange</t>
+          <t>(S)-Malate_c__Day_sp_exchange</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1.073623309526004</v>
+        <v>1.07362330952184</v>
       </c>
       <c r="C19" t="n">
-        <v>0.9911678333352476</v>
+        <v>0.9911678333325844</v>
       </c>
       <c r="D19" t="n">
-        <v>9.399136999984796</v>
+        <v>9.399137000000328</v>
       </c>
       <c r="E19" t="b">
         <v>1</v>
@@ -800,17 +800,17 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Fumarate_Day_sp_exchange</t>
+          <t>Fumarate__Day_sp_exchange</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.0009240000000030056</v>
+        <v>0.000923999999994571</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.03814799999999672</v>
+        <v>-0.03814799999996859</v>
       </c>
       <c r="D20" t="n">
-        <v>0.03814799999988958</v>
+        <v>0.03814800000000404</v>
       </c>
       <c r="E20" t="b">
         <v>0</v>

</xml_diff>